<commit_message>
some more test cases added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Frameworks\playwright-cucumber-framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E2E01B-18E8-4432-B0BD-A3BCACD3A4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4E6574-6536-4719-9699-B271D12A3FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ApplicationCheck" sheetId="1" r:id="rId1"/>
+    <sheet name="SauceDemoShop" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>Smoke</t>
   </si>
@@ -46,6 +47,36 @@
   </si>
   <si>
     <t>Regression</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>productName</t>
   </si>
 </sst>
 </file>
@@ -363,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,9 +405,10 @@
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -386,8 +418,20 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -397,8 +441,20 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>12345</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -407,6 +463,103 @@
       </c>
       <c r="C3" t="s">
         <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>54321</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7254589-B9F5-45F2-BF54-ECA13D79A198}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>12345</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>54321</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>